<commit_message>
05_TSA (CÓDIGO ESTABLE PARA LA EXTRACCIÓN)
Se configura el código para la extracción de la información y se hace el etiquetado respectivo de la ED.
</commit_message>
<xml_diff>
--- a/05_TSA/01_Código_Extracción/04_Resultados/Estructura_Datos/HOJA_INGRESOS_ORI_2024.xlsx
+++ b/05_TSA/01_Código_Extracción/04_Resultados/Estructura_Datos/HOJA_INGRESOS_ORI_2024.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t xml:space="preserve">Archivo</t>
   </si>
@@ -62,7 +62,10 @@
     <t xml:space="preserve">Entre núcleos de población ejidal o comunal y pequeños propietarios</t>
   </si>
   <si>
-    <t xml:space="preserve">Entre núcleos de población ejidal o comunal y sociedades</t>
+    <t xml:space="preserve">Entre núcleos de población ejidal o comunal y sociedades o asociaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entre núcleos de población ejidal o comunal y colonia agrícola que adopta dominio pleno </t>
   </si>
   <si>
     <t xml:space="preserve">Subtotal de asuntos por restitución de tierras, bosques y aguas a núcleos de población o a sus integrantes</t>
@@ -152,16 +155,19 @@
     <t xml:space="preserve">3431050</t>
   </si>
   <si>
+    <t xml:space="preserve">Diciembre/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Archivo_EST-34A.xls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tribunal Unitario Agrario Distrito 34-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34-A04002</t>
+  </si>
+  <si>
     <t xml:space="preserve">DICIEMBRE/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Archivo_EST-34A.xls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tribunal Unitario Agrario Distrito 34-A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34-A04002</t>
   </si>
 </sst>
 </file>
@@ -623,19 +629,22 @@
       <c r="AQ1" t="s">
         <v>42</v>
       </c>
+      <c r="AR1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E2" t="n">
         <v>141</v>
@@ -662,7 +671,7 @@
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="N2" t="n">
         <v>0</v>
@@ -680,7 +689,7 @@
         <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T2" t="n">
         <v>0</v>
@@ -707,10 +716,10 @@
         <v>1</v>
       </c>
       <c r="AB2" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AC2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD2" t="n">
         <v>4</v>
@@ -719,11 +728,11 @@
         <v>0</v>
       </c>
       <c r="AF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG2" t="n">
         <v>103</v>
       </c>
-      <c r="AG2" t="n">
-        <v>0</v>
-      </c>
       <c r="AH2" t="n">
         <v>0</v>
       </c>
@@ -749,24 +758,27 @@
         <v>0</v>
       </c>
       <c r="AP2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ2" t="n">
         <v>2</v>
       </c>
-      <c r="AQ2" t="n">
+      <c r="AR2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E3" t="n">
         <v>141</v>
@@ -793,7 +805,7 @@
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="N3" t="n">
         <v>0</v>
@@ -811,7 +823,7 @@
         <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3" t="n">
         <v>0</v>
@@ -838,10 +850,10 @@
         <v>1</v>
       </c>
       <c r="AB3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AC3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD3" t="n">
         <v>4</v>
@@ -850,11 +862,11 @@
         <v>0</v>
       </c>
       <c r="AF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG3" t="n">
         <v>103</v>
       </c>
-      <c r="AG3" t="n">
-        <v>0</v>
-      </c>
       <c r="AH3" t="n">
         <v>0</v>
       </c>
@@ -880,9 +892,12 @@
         <v>0</v>
       </c>
       <c r="AP3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ3" t="n">
         <v>2</v>
       </c>
-      <c r="AQ3" t="n">
+      <c r="AR3" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>